<commit_message>
Table c: extracted, cleaned, and exported into csv file
</commit_message>
<xml_diff>
--- a/Clinical_Research_Field_List.xlsx
+++ b/Clinical_Research_Field_List.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gahyo\Documents\Datacamp\Final_Project\Clinical_Trials_Research_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FACCFC7B-0016-48B7-805E-BD2C89958869}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DB0E8C0-38D3-49E3-AB66-9594CF10C8AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16125" yWindow="0" windowWidth="22380" windowHeight="20985" xr2:uid="{BA23B5C0-076B-4CA7-A678-6667A5D57DFD}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{BA23B5C0-076B-4CA7-A678-6667A5D57DFD}"/>
   </bookViews>
   <sheets>
     <sheet name="Field List" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Field List'!$B$2:$C$30</definedName>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="64">
   <si>
     <t>Brief Title</t>
   </si>
@@ -223,6 +224,15 @@
   </si>
   <si>
     <t>ALL</t>
+  </si>
+  <si>
+    <t>c*</t>
+  </si>
+  <si>
+    <t>StartDate</t>
+  </si>
+  <si>
+    <t>CompletionDate</t>
   </si>
 </sst>
 </file>
@@ -279,7 +289,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -294,7 +304,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -613,7 +622,7 @@
   <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -750,14 +759,14 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="6" t="s">
         <v>54</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>21</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -786,7 +795,7 @@
       <c r="A16" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" t="s">
         <v>42</v>
       </c>
       <c r="C16" s="5" t="s">
@@ -945,4 +954,76 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A03616C-6752-4B6A-938E-73E040255A68}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A55" sqref="A55"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="56.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="str">
+        <f>A1</f>
+        <v>OrgStudyId</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" t="str">
+        <f>_xlfn.CONCAT(B1,",",A2)</f>
+        <v>OrgStudyId,BriefTitle</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" t="str">
+        <f t="shared" ref="B3:B6" si="0">_xlfn.CONCAT(B2,",",A3)</f>
+        <v>OrgStudyId,BriefTitle,StartDate</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" t="str">
+        <f t="shared" si="0"/>
+        <v>OrgStudyId,BriefTitle,StartDate,CompletionDate</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v>OrgStudyId,BriefTitle,StartDate,CompletionDate,OverallStatus</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" t="str">
+        <f t="shared" si="0"/>
+        <v>OrgStudyId,BriefTitle,StartDate,CompletionDate,OverallStatus,StudyType</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>